<commit_message>
Script for code gen stage 1
</commit_message>
<xml_diff>
--- a/Software-Requirements/BIT/Phase Tests Requirements.xlsx
+++ b/Software-Requirements/BIT/Phase Tests Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Programming\Ada\System Checks\Software Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Programming\Ada\System Checks\Software-Requirements\BIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B87A6FD-DEA6-4A6D-8F06-C7793325A874}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2EFEBF8-3A7B-4FEB-AFB3-C8D9E4C034E7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,11 @@
     <sheet name="Procedures Section" sheetId="1" r:id="rId1"/>
     <sheet name="Section Statistics" sheetId="3" r:id="rId2"/>
     <sheet name="Tests Section" sheetId="2" r:id="rId3"/>
+    <sheet name="Range Types" sheetId="4" r:id="rId4"/>
+    <sheet name="Boolean" sheetId="5" r:id="rId5"/>
+    <sheet name="Enum Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Array Types" sheetId="7" r:id="rId7"/>
+    <sheet name="Constants" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tests Section'!$A$1:$M$339</definedName>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="642">
   <si>
     <t>Procedure</t>
   </si>
@@ -1873,9 +1878,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>DescrIBITion</t>
-  </si>
-  <si>
     <t>IBIT</t>
   </si>
   <si>
@@ -1892,13 +1894,520 @@
   </si>
   <si>
     <t>general_checks</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Call_Failure</t>
+  </si>
+  <si>
+    <t>Call_Failure_And_Details</t>
+  </si>
+  <si>
+    <t>Failures_Status</t>
+  </si>
+  <si>
+    <t>Abort</t>
+  </si>
+  <si>
+    <t>Log_Failure</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Read_1_Bit_Signal_Data</t>
+  </si>
+  <si>
+    <t>Read_8_Bit_Signal_Data</t>
+  </si>
+  <si>
+    <t>Read_16_Bit_Signal_Data</t>
+  </si>
+  <si>
+    <t>Read_Register_Contents</t>
+  </si>
+  <si>
+    <t>Read_Signal_To_Register_Data</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Initialise_Engager</t>
+  </si>
+  <si>
+    <t>Stage_Run</t>
+  </si>
+  <si>
+    <t>Get_Release_State</t>
+  </si>
+  <si>
+    <t>Comms_Rx_Recieve</t>
+  </si>
+  <si>
+    <t>Comms_Tx_Send</t>
+  </si>
+  <si>
+    <t>Get_Weapon_Code_Lock</t>
+  </si>
+  <si>
+    <t>Read_And_Buffer_Sensor_Data</t>
+  </si>
+  <si>
+    <t>Porobability_Lock_Failure</t>
+  </si>
+  <si>
+    <t>Monitor_Log</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Get_Impact</t>
+  </si>
+  <si>
+    <t>Release_Device</t>
+  </si>
+  <si>
+    <t>Count_Begin</t>
+  </si>
+  <si>
+    <t>Explosion_Launch</t>
+  </si>
+  <si>
+    <t>Select_Target</t>
+  </si>
+  <si>
+    <t>Get_Count</t>
+  </si>
+  <si>
+    <t>Configuration_Constructor</t>
+  </si>
+  <si>
+    <t>Test_Id Local = Test_Id
+If Failure_Data_Structure(Tests_Id_Local) = True
+    return True
+else 
+    return False
+end if</t>
+  </si>
+  <si>
+    <t>If Failure_Key = TRUE
+    for range of Failure_List loop
+          If Test_Id = Failure_List(Index) .Value(TRUE)
+              Details_Record = Failure_List_Details(Index)
+          End if
+   End Loop
+End if</t>
+  </si>
+  <si>
+    <t>If Failure_Key = TRUE
+    Project_Main_End(TRUE)
+End if</t>
+  </si>
+  <si>
+    <t>If Failure_Key = TRUE
+    Failure_List(Test_Id).Value = True
+    Failure_List_Details(Index) = Details_Record 
+End if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Register, Bit)  = Read_Bit_Register_Contents(Signal_Name)
+Register_Value = Read_Signal_To_Register_Data(Register, Bit)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Register, Bits)  = Read_Register_Contents(Signal_Name)
+Register_Value = Read_Signal_To_Register_Data(Register, Bits)
+</t>
+  </si>
+  <si>
+    <t>Register = Register_Array(Signal)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Set all Package values to default</t>
+  </si>
+  <si>
+    <t>If Stage_Recieve
+         (Address_1, Value_1) = Comms_Tx_Recieve
+         (Address_2, Value_2) = 
+         Read_And_Buffer_Sensor_Data(Address_1, Value_1)
+         If Value &gt;= Constant 
+               Comms_Rx_Send(Address_2, Value_2)
+End If</t>
+  </si>
+  <si>
+    <t>When Code_Check_Key = TRUE
+          While Timer &lt; Constant_1
+                    State = Get_Release_State(Weapon_Code)
+End When</t>
+  </si>
+  <si>
+    <t>When Trigger_Monitor_Signal = TRUE
+          While Timer &lt; Constant_1
+                    Monitor_Clear_Run = True
+                    Wait for Delay_1
+                    Stage_Monitor()
+           End loop
+           Monitor_Restart = True
+           If x = Monitor_Run() = TRUE
+                 Trigger_Monitor_Signal = FALSE
+           End if
+End When</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage = Pre_Start
+case Pre_Start:
+      Start_Countdown = Count_Begin(Simulation_Id)
+      Explosition_Count = Explosion_Launch
+      if Start_Countdown = True
+          Target_Variable  = Select_Target(Input)
+          Stage = Count_Release
+      end if
+case Count_Release:
+      Countdown_Release = Get_Count
+      if Countdown_Release = True
+            x = Release_Device(Target_Variable)
+            if Explosion_Count is = x
+                Stage = Get_Impact_Coverage
+            else 
+                Stage = Pre_Start
+            end if
+      end if
+case Get_Impact_Coverage:
+       if Get_Impact(Target_Variable,  
+                                Explosion_Count) = Target_Area 
+            Density = Density + Density_Change
+            Radius = Radius - Radius_Change
+       else 
+            Density = Density - Density_Change
+            Radius = Radius + Radius_Change
+end switch
+</t>
+  </si>
+  <si>
+    <t>Return Target_Variable * Explosion_Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Target_Variable &lt; 50
+    Return_Value = 1
+else if Target_Variable &lt; 100 and &gt; 50
+      Return_Value = 2
+else if Target_Variable &lt; 150 and &gt; 100
+      Return_Value = 3
+else if Target_Variable &lt; 200 and &gt; 150
+      Return_Value = 4
+else if Target_Variable &lt; 400
+      Return_Value = 5
+else
+      Return_Value = 6
+end if
+</t>
+  </si>
+  <si>
+    <t>If Simulation_Id'Valid   
+    return True
+else
+    return False
+end if</t>
+  </si>
+  <si>
+    <t>Return Random(Value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Input'Valid
+    return Value = (Input * 50) - 100
+else 
+     return 0
+end if </t>
+  </si>
+  <si>
+    <t xml:space="preserve">While Timer &lt; Time_Constant_1 loop
+   for Range of Count_Array loop
+      if Count_Array(Index) &lt; Cnt_Acc_Tmr_Cons 
+          Count_Failure_Array(Index) = True
+          Exit_Loop = True
+      else
+          Count_Failure_Array(Index) = False
+      end if
+   end loop 
+End Loop
+If Exit_Loop = True
+   Return False
+else
+   Return True
+End if </t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Input a test Id to see if a failure occurred</t>
+  </si>
+  <si>
+    <t>Input a test Id to see if a failure occurred and all occurrence details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outputs a list of all failures for last run time </t>
+  </si>
+  <si>
+    <t>Shuts down all operations and logs all details</t>
+  </si>
+  <si>
+    <t>Logs a failure for the Test Id entered</t>
+  </si>
+  <si>
+    <t>Reads the signal value and returns a boolean</t>
+  </si>
+  <si>
+    <t>Reads the signal value and returns a 8 bit value</t>
+  </si>
+  <si>
+    <t>Reads the signal value and returns a 16 bit value</t>
+  </si>
+  <si>
+    <t>Returns the contents of the register indexed by what bits are needed</t>
+  </si>
+  <si>
+    <t>Reads the register value for the signal entered</t>
+  </si>
+  <si>
+    <t>Initialises variables for the engage run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starts Monitor set values </t>
+  </si>
+  <si>
+    <t>Returns the release state of GPIO components</t>
+  </si>
+  <si>
+    <t>Case statement for receiving 64 bit messages</t>
+  </si>
+  <si>
+    <t>Case statement for sending 64 bit messages</t>
+  </si>
+  <si>
+    <t>Returns the state of various weapon states</t>
+  </si>
+  <si>
+    <t>Loads input sensor data to data structure</t>
+  </si>
+  <si>
+    <t>Calculates probability of all phase failures</t>
+  </si>
+  <si>
+    <t>Clears and restarts the monitor</t>
+  </si>
+  <si>
+    <t>Sets the density and radius of the Device</t>
+  </si>
+  <si>
+    <t>Returns a area squared</t>
+  </si>
+  <si>
+    <t>Outputs a time based of explosion pin for explosion count check</t>
+  </si>
+  <si>
+    <t>Starts the Count</t>
+  </si>
+  <si>
+    <t>Sets a random output from 0 to 6</t>
+  </si>
+  <si>
+    <t>From a target input, the function selects a target variable from a array</t>
+  </si>
+  <si>
+    <t>Returns a failure in the count if it occurs one in a loop</t>
+  </si>
+  <si>
+    <t>Initialises Variables for different device settings</t>
+  </si>
+  <si>
+    <t>Signal Traces</t>
+  </si>
+  <si>
+    <t>Code_Check_Key = Code_Check_Key_Type
+Weapon_Code = Weapon_Code_Type
+State = Weapon_Code_Lock_State_Type</t>
+  </si>
+  <si>
+    <t>Trigger_Monitor_Signal = Boolean
+Timer, Constant_1, Delay_1= Timer_Millis_Type
+Constant_1 = Timer_Cons_Lock
+Delay_1 = Time_Dly_001
+Monitor_Clear_Run = Monitor_Clear_Run_Type</t>
+  </si>
+  <si>
+    <t>Target_Variable = Sel_Target_Type
+Explosion_Count = Explosion_Launch_Type</t>
+  </si>
+  <si>
+    <t>Target_Variable = Sel_Target_Type
+Return = Explosion_Launch_Type</t>
+  </si>
+  <si>
+    <t>Simulation_Id = Simulation_Id_Type</t>
+  </si>
+  <si>
+    <t>Value = Explosion_Launch_Type</t>
+  </si>
+  <si>
+    <t>Input = Target_Axis_Type
+Value = Sel_Target_Type</t>
+  </si>
+  <si>
+    <t>Timer= Timer_Millis_Type
+Timer_Constant_1 = Timer_Cons_Lock
+Count_Array = Count_Array_Type
+Index = Count_Array_Index_Type
+Cnt_Acc_Tmr_Cons = Count_Value_Type
+Count_Failure_Array = Count_Failure_Array_Type
+Exit_Loop = Boolean</t>
+  </si>
+  <si>
+    <t>Count_Value_Type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Count_Array_Index_Type</t>
+  </si>
+  <si>
+    <t>Timer_Millis_Type</t>
+  </si>
+  <si>
+    <t>Sel_Target_Type</t>
+  </si>
+  <si>
+    <t>Target_Axis_Type</t>
+  </si>
+  <si>
+    <t>Explosion_Launch_Type</t>
+  </si>
+  <si>
+    <t>Parent_Hex_Subtype</t>
+  </si>
+  <si>
+    <t>Parent_Hex</t>
+  </si>
+  <si>
+    <t>Subtype</t>
+  </si>
+  <si>
+    <t>Range Max</t>
+  </si>
+  <si>
+    <t>Range Min</t>
+  </si>
+  <si>
+    <t>Type Name</t>
+  </si>
+  <si>
+    <t>Parent Type</t>
+  </si>
+  <si>
+    <t>Type or Subtype</t>
+  </si>
+  <si>
+    <t>Package Name</t>
+  </si>
+  <si>
+    <t>Monitor_Clear_Run_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_10101000
+</t>
+  </si>
+  <si>
+    <t>Simulation_Id_Type</t>
+  </si>
+  <si>
+    <t>Round_Fail_5</t>
+  </si>
+  <si>
+    <t>Round_Fail_4</t>
+  </si>
+  <si>
+    <t>Round_Fail_3</t>
+  </si>
+  <si>
+    <t>Round_Fail_2</t>
+  </si>
+  <si>
+    <t>Round_Fail_1</t>
+  </si>
+  <si>
+    <t>Round_Fail_Check</t>
+  </si>
+  <si>
+    <t>No Of Values</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Count_Failure_Array_Type</t>
+  </si>
+  <si>
+    <t>Count_Array_Type</t>
+  </si>
+  <si>
+    <t>Mask_Index_Array_Type</t>
+  </si>
+  <si>
+    <t>Mask_Type</t>
+  </si>
+  <si>
+    <t>Array Values Type</t>
+  </si>
+  <si>
+    <t>Index Type</t>
+  </si>
+  <si>
+    <t>Timer_Dly_001</t>
+  </si>
+  <si>
+    <t>Timer_Cons_Lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cnt_Knk_Tmr_Cons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cnt_Act_Tmr_Cons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cnt_Rej_Tmr_Cons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cnt_Acc_Tmr_Cons </t>
+  </si>
+  <si>
+    <t>Hex_Value_Lock</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Constant Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1924,8 +2433,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1948,6 +2471,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2031,7 +2560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2085,6 +2614,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2381,25 +2928,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2413,7 +2960,7 @@
         <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>506</v>
+        <v>562</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>98</v>
@@ -2422,12 +2969,15 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>178</v>
@@ -2438,7 +2988,9 @@
       <c r="D2" s="18">
         <v>10101000</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="22" t="s">
+        <v>563</v>
+      </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2446,10 +2998,11 @@
         <v>7</v>
       </c>
       <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>178</v>
@@ -2460,18 +3013,21 @@
       <c r="D3" s="18">
         <v>10102000</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="22" t="s">
+        <v>564</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>8</v>
@@ -2482,18 +3038,21 @@
       <c r="D4" s="18">
         <v>10201000</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="22" t="s">
+        <v>565</v>
+      </c>
       <c r="F4" s="5">
         <v>2</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H4" s="19"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>8</v>
@@ -2504,18 +3063,21 @@
       <c r="D5" s="18">
         <v>10202000</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="22" t="s">
+        <v>566</v>
+      </c>
       <c r="F5" s="5">
         <v>2</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H5" s="19"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>8</v>
@@ -2526,18 +3088,21 @@
       <c r="D6" s="18">
         <v>10203000</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="22" t="s">
+        <v>567</v>
+      </c>
       <c r="F6" s="5">
         <v>2</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H6" s="19"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>9</v>
@@ -2548,18 +3113,21 @@
       <c r="D7" s="18">
         <v>10301000</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="22" t="s">
+        <v>568</v>
+      </c>
       <c r="F7" s="5">
         <v>3</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H7" s="19"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>9</v>
@@ -2570,18 +3138,21 @@
       <c r="D8" s="18">
         <v>10302000</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="22" t="s">
+        <v>569</v>
+      </c>
       <c r="F8" s="5">
         <v>3</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="19"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>9</v>
@@ -2592,18 +3163,21 @@
       <c r="D9" s="18">
         <v>10303000</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="22" t="s">
+        <v>570</v>
+      </c>
       <c r="F9" s="5">
         <v>4</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="19"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>9</v>
@@ -2614,18 +3188,21 @@
       <c r="D10" s="18">
         <v>10304000</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="22" t="s">
+        <v>571</v>
+      </c>
       <c r="F10" s="5">
         <v>1</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H10" s="19"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>9</v>
@@ -2636,18 +3213,21 @@
       <c r="D11" s="18">
         <v>10305000</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="22" t="s">
+        <v>572</v>
+      </c>
       <c r="F11" s="5">
         <v>3</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H11" s="19"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>30</v>
@@ -2658,18 +3238,21 @@
       <c r="D12" s="18">
         <v>10401000</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="22" t="s">
+        <v>573</v>
+      </c>
       <c r="F12" s="5">
         <v>2</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="19"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>30</v>
@@ -2680,18 +3263,21 @@
       <c r="D13" s="18">
         <v>10402000</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="22" t="s">
+        <v>574</v>
+      </c>
       <c r="F13" s="5">
         <v>3</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="19"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
@@ -2702,18 +3288,21 @@
       <c r="D14" s="18">
         <v>10403000</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="22" t="s">
+        <v>575</v>
+      </c>
       <c r="F14" s="5">
         <v>5</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H14" s="19"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>31</v>
@@ -2724,18 +3313,21 @@
       <c r="D15" s="18">
         <v>10501000</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="22" t="s">
+        <v>576</v>
+      </c>
       <c r="F15" s="5">
         <v>3</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H15" s="19"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>31</v>
@@ -2746,18 +3338,21 @@
       <c r="D16" s="18">
         <v>10502000</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="22" t="s">
+        <v>577</v>
+      </c>
       <c r="F16" s="5">
         <v>3</v>
       </c>
       <c r="G16" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H16" s="19"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>31</v>
@@ -2768,18 +3363,21 @@
       <c r="D17" s="18">
         <v>10503000</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="22" t="s">
+        <v>578</v>
+      </c>
       <c r="F17" s="5">
         <v>4</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H17" s="19"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>31</v>
@@ -2790,18 +3388,21 @@
       <c r="D18" s="18">
         <v>10504000</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="22" t="s">
+        <v>579</v>
+      </c>
       <c r="F18" s="5">
         <v>4</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H18" s="19"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>31</v>
@@ -2812,18 +3413,21 @@
       <c r="D19" s="18">
         <v>10505000</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="22" t="s">
+        <v>580</v>
+      </c>
       <c r="F19" s="5">
         <v>3</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="19"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>178</v>
@@ -2834,16 +3438,19 @@
       <c r="D20" s="18">
         <v>20101000</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="22" t="s">
+        <v>581</v>
+      </c>
       <c r="F20" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>178</v>
@@ -2854,16 +3461,19 @@
       <c r="D21" s="18">
         <v>20102000</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="22" t="s">
+        <v>582</v>
+      </c>
       <c r="F21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>187</v>
@@ -2874,18 +3484,21 @@
       <c r="D22" s="18">
         <v>20201000</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="22" t="s">
+        <v>583</v>
+      </c>
       <c r="F22" s="5">
         <v>2</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="19"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>187</v>
@@ -2896,18 +3509,21 @@
       <c r="D23" s="18">
         <v>20202000</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="22" t="s">
+        <v>584</v>
+      </c>
       <c r="F23" s="5">
         <v>2</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="19"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>187</v>
@@ -2918,18 +3534,21 @@
       <c r="D24" s="18">
         <v>20203000</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="22" t="s">
+        <v>585</v>
+      </c>
       <c r="F24" s="5">
         <v>5</v>
       </c>
       <c r="G24" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="19"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>187</v>
@@ -2940,18 +3559,21 @@
       <c r="D25" s="18">
         <v>20204000</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="22" t="s">
+        <v>586</v>
+      </c>
       <c r="F25" s="5">
         <v>5</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="19"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>187</v>
@@ -2962,18 +3584,21 @@
       <c r="D26" s="18">
         <v>20205000</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="22" t="s">
+        <v>587</v>
+      </c>
       <c r="F26" s="5">
         <v>3</v>
       </c>
       <c r="G26" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H26" s="19"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>45</v>
@@ -2984,18 +3609,21 @@
       <c r="D27" s="18">
         <v>20301000</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="22" t="s">
+        <v>588</v>
+      </c>
       <c r="F27" s="5">
         <v>2</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H27" s="19"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>45</v>
@@ -3006,18 +3634,21 @@
       <c r="D28" s="18">
         <v>20302000</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="22" t="s">
+        <v>589</v>
+      </c>
       <c r="F28" s="5">
         <v>3</v>
       </c>
       <c r="G28" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H28" s="19"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>45</v>
@@ -3035,11 +3666,12 @@
       <c r="G29" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H29" s="19"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>45</v>
@@ -3057,11 +3689,12 @@
       <c r="G30" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H30" s="19"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>45</v>
@@ -3079,11 +3712,12 @@
       <c r="G31" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H31" s="19"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>45</v>
@@ -3101,11 +3735,12 @@
       <c r="G32" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H32" s="19"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>45</v>
@@ -3123,11 +3758,12 @@
       <c r="G33" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H33" s="19"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>60</v>
@@ -3145,11 +3781,12 @@
       <c r="G34" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="19"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>60</v>
@@ -3163,13 +3800,14 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="5" t="s">
+      <c r="H35" s="19"/>
+      <c r="I35" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>60</v>
@@ -3183,13 +3821,14 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="5" t="s">
+      <c r="H36" s="19"/>
+      <c r="I36" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>60</v>
@@ -3203,13 +3842,14 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="19"/>
+      <c r="I37" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>65</v>
@@ -3227,11 +3867,12 @@
       <c r="G38" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="H38" s="19"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>65</v>
@@ -3249,11 +3890,12 @@
       <c r="G39" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H39" s="19"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>65</v>
@@ -3271,11 +3913,12 @@
       <c r="G40" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H40" s="19"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>68</v>
@@ -3293,11 +3936,12 @@
       <c r="G41" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H41" s="19"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>68</v>
@@ -3315,11 +3959,12 @@
       <c r="G42" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H42" s="19"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>68</v>
@@ -3337,11 +3982,12 @@
       <c r="G43" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="19"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>178</v>
@@ -3357,11 +4003,12 @@
         <v>7</v>
       </c>
       <c r="G44" s="19"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="19"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>178</v>
@@ -3377,11 +4024,12 @@
         <v>7</v>
       </c>
       <c r="G45" s="19"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H45" s="19"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>185</v>
@@ -3399,11 +4047,12 @@
       <c r="G46" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H46" s="19"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>185</v>
@@ -3421,11 +4070,12 @@
       <c r="G47" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H47" s="19"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>185</v>
@@ -3443,11 +4093,12 @@
       <c r="G48" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H48" s="19"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>185</v>
@@ -3465,11 +4116,12 @@
       <c r="G49" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="H49" s="19"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>185</v>
@@ -3487,11 +4139,12 @@
       <c r="G50" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="H50" s="19"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>185</v>
@@ -3509,11 +4162,12 @@
       <c r="G51" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="H51" s="19"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>185</v>
@@ -3531,11 +4185,12 @@
       <c r="G52" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H52" s="19"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>185</v>
@@ -3553,11 +4208,12 @@
       <c r="G53" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H53" s="19"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>185</v>
@@ -3575,11 +4231,12 @@
       <c r="G54" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H54" s="19"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>196</v>
@@ -3597,11 +4254,12 @@
       <c r="G55" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H55" s="19"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>79</v>
@@ -3619,11 +4277,12 @@
       <c r="G56" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H56" s="19"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>79</v>
@@ -3641,11 +4300,12 @@
       <c r="G57" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H57" s="19"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>79</v>
@@ -3663,11 +4323,12 @@
       <c r="G58" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="19"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>178</v>
@@ -3683,11 +4344,12 @@
         <v>7</v>
       </c>
       <c r="G59" s="19"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="19"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>178</v>
@@ -3703,11 +4365,12 @@
         <v>7</v>
       </c>
       <c r="G60" s="19"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H60" s="19"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>83</v>
@@ -3725,11 +4388,12 @@
       <c r="G61" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H61" s="19"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>84</v>
@@ -3747,11 +4411,12 @@
       <c r="G62" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="H62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H62" s="19"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>84</v>
@@ -3769,11 +4434,12 @@
       <c r="G63" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H63" s="19"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>84</v>
@@ -3791,11 +4457,12 @@
       <c r="G64" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H64" s="19"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>188</v>
@@ -3813,11 +4480,12 @@
       <c r="G65" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H65" s="19"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>188</v>
@@ -3835,11 +4503,12 @@
       <c r="G66" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H66" s="19"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B67" s="20" t="s">
         <v>188</v>
@@ -3857,11 +4526,12 @@
       <c r="G67" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H67" s="19"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>188</v>
@@ -3879,11 +4549,12 @@
       <c r="G68" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H68" s="19"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>176</v>
@@ -3901,11 +4572,12 @@
       <c r="G69" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H69" s="19"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>176</v>
@@ -3923,11 +4595,12 @@
       <c r="G70" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H70" s="19"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>176</v>
@@ -3945,11 +4618,12 @@
       <c r="G71" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H71" s="19"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>176</v>
@@ -3967,11 +4641,12 @@
       <c r="G72" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H72" s="19"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>176</v>
@@ -3989,11 +4664,12 @@
       <c r="G73" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="H73" s="5"/>
-    </row>
-    <row r="74" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H73" s="19"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>176</v>
@@ -4011,11 +4687,12 @@
       <c r="G74" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H74" s="19"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>176</v>
@@ -4033,11 +4710,12 @@
       <c r="G75" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="H75" s="5"/>
-    </row>
-    <row r="76" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H75" s="19"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>176</v>
@@ -4055,11 +4733,12 @@
       <c r="G76" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="H76" s="5"/>
-    </row>
-    <row r="77" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H76" s="19"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>176</v>
@@ -4077,11 +4756,12 @@
       <c r="G77" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="H77" s="5"/>
-    </row>
-    <row r="78" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H77" s="19"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>176</v>
@@ -4099,11 +4779,12 @@
       <c r="G78" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="H78" s="5"/>
-    </row>
-    <row r="79" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H78" s="19"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>176</v>
@@ -4121,11 +4802,12 @@
       <c r="G79" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="H79" s="5"/>
-    </row>
-    <row r="80" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="H79" s="19"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>176</v>
@@ -4143,11 +4825,12 @@
       <c r="G80" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="H80" s="5"/>
-    </row>
-    <row r="81" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="H80" s="19"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>176</v>
@@ -4165,11 +4848,12 @@
       <c r="G81" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="H81" s="5"/>
-    </row>
-    <row r="82" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="H81" s="19"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>176</v>
@@ -4187,11 +4871,12 @@
       <c r="G82" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="H82" s="5"/>
-    </row>
-    <row r="83" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H82" s="19"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>30</v>
@@ -4209,11 +4894,12 @@
       <c r="G83" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="H83" s="5"/>
-    </row>
-    <row r="84" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="H83" s="19"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>30</v>
@@ -4231,11 +4917,12 @@
       <c r="G84" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="H84" s="5"/>
-    </row>
-    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H84" s="19"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>30</v>
@@ -4253,11 +4940,12 @@
       <c r="G85" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H85" s="5"/>
-    </row>
-    <row r="86" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H85" s="19"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>30</v>
@@ -4275,11 +4963,12 @@
       <c r="G86" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="H86" s="5"/>
-    </row>
-    <row r="87" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H86" s="19"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>30</v>
@@ -4297,11 +4986,12 @@
       <c r="G87" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="H87" s="5"/>
-    </row>
-    <row r="88" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H87" s="19"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>30</v>
@@ -4319,11 +5009,12 @@
       <c r="G88" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="H88" s="5"/>
-    </row>
-    <row r="89" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="H88" s="19"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>179</v>
@@ -4341,11 +5032,12 @@
       <c r="G89" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="H89" s="5"/>
-    </row>
-    <row r="90" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="H89" s="19"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>179</v>
@@ -4363,11 +5055,12 @@
       <c r="G90" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="H90" s="5"/>
-    </row>
-    <row r="91" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H90" s="19"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>50</v>
@@ -4385,11 +5078,12 @@
       <c r="G91" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H91" s="5"/>
-    </row>
-    <row r="92" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H91" s="19"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>50</v>
@@ -4407,11 +5101,12 @@
       <c r="G92" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H92" s="5"/>
-    </row>
-    <row r="93" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H92" s="19"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>50</v>
@@ -4429,11 +5124,12 @@
       <c r="G93" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H93" s="5"/>
-    </row>
-    <row r="94" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="H93" s="19"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>53</v>
@@ -4451,11 +5147,12 @@
       <c r="G94" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="H94" s="5"/>
-    </row>
-    <row r="95" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H94" s="19"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>53</v>
@@ -4473,11 +5170,12 @@
       <c r="G95" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="H95" s="5"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="19"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>53</v>
@@ -4493,13 +5191,14 @@
         <v>2</v>
       </c>
       <c r="G96" s="19"/>
-      <c r="H96" s="5" t="s">
+      <c r="H96" s="19"/>
+      <c r="I96" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>53</v>
@@ -4517,11 +5216,12 @@
       <c r="G97" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="H97" s="5"/>
-    </row>
-    <row r="98" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H97" s="19"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>53</v>
@@ -4539,11 +5239,12 @@
       <c r="G98" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="H98" s="5"/>
-    </row>
-    <row r="99" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H98" s="19"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>53</v>
@@ -4561,11 +5262,12 @@
       <c r="G99" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="H99" s="5"/>
-    </row>
-    <row r="100" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H99" s="19"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B100" s="17" t="s">
         <v>175</v>
@@ -4583,11 +5285,12 @@
       <c r="G100" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="H100" s="5"/>
-    </row>
-    <row r="101" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="H100" s="19"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B101" s="17" t="s">
         <v>175</v>
@@ -4605,11 +5308,12 @@
       <c r="G101" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="H101" s="5"/>
-    </row>
-    <row r="102" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="H101" s="19"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B102" s="17" t="s">
         <v>175</v>
@@ -4627,97 +5331,426 @@
       <c r="G102" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="H102" s="5"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G103" s="3"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G104" s="3"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G105" s="3"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G106" s="3"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G107" s="3"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G108" s="3"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G109" s="3"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G110" s="3"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G111" s="3"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G112" s="3"/>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G113" s="3"/>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G114" s="3"/>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G115" s="3"/>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G116" s="3"/>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G117" s="3"/>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G118" s="3"/>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G119" s="3"/>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G120" s="3"/>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G121" s="3"/>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G122" s="3"/>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G123" s="3"/>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G124" s="3"/>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G125" s="3"/>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G127" s="3"/>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G128" s="3"/>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="19"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="1:9" ht="102.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="C103" s="21" t="s">
+        <v>513</v>
+      </c>
+      <c r="G103" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:9" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="C104" s="21" t="s">
+        <v>514</v>
+      </c>
+      <c r="G104" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>515</v>
+      </c>
+      <c r="G105" s="22"/>
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="C106" s="21" t="s">
+        <v>516</v>
+      </c>
+      <c r="G106" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:9" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="G107" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="C108" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="G108" s="23" t="s">
+        <v>546</v>
+      </c>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="C109" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="G109" s="23" t="s">
+        <v>547</v>
+      </c>
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="G110" s="23" t="s">
+        <v>547</v>
+      </c>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="G111" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="G112" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="G113" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="G114" s="22" t="s">
+        <v>551</v>
+      </c>
+      <c r="H114" s="3"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>527</v>
+      </c>
+      <c r="G115" s="22"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B116" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>528</v>
+      </c>
+      <c r="G116" s="22"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>529</v>
+      </c>
+      <c r="G117" s="22"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B118" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="G118" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B119" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="G119" s="22"/>
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="G120" s="22"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" ht="179.25" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>524</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>533</v>
+      </c>
+      <c r="G121" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="H121" s="22" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C122" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="G122" s="25" t="s">
+        <v>554</v>
+      </c>
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="G123" s="25" t="s">
+        <v>555</v>
+      </c>
+      <c r="H123" s="22" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="229.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B124" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="G124" s="25" t="s">
+        <v>556</v>
+      </c>
+      <c r="H124" s="22" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="G125" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="H125" s="22" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="G126" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="H126" s="22" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A127" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G127" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="H127" s="22" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="243" x14ac:dyDescent="0.25">
+      <c r="A128" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C128" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="G128" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="H128" s="22" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B129" s="21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>541</v>
+      </c>
       <c r="G129" s="3"/>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G130" s="3"/>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H130" s="3"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G131" s="3"/>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H131" s="3"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4749,16 +5782,16 @@
         <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>89</v>
@@ -4767,7 +5800,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTA('Procedures Section'!C:C)</f>
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="B2">
         <f>COUNTIF('Procedures Section'!$A:$A,B1)</f>
@@ -5470,7 +6503,7 @@
         <v>10101000</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>178</v>
@@ -5493,7 +6526,7 @@
         <v>10102000</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>178</v>
@@ -5516,7 +6549,7 @@
         <v>10201000</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>8</v>
@@ -5549,7 +6582,7 @@
         <v>10202000</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>8</v>
@@ -5582,7 +6615,7 @@
         <v>10203000</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>8</v>
@@ -5615,7 +6648,7 @@
         <v>10203001</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>8</v>
@@ -5648,7 +6681,7 @@
         <v>10301000</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>9</v>
@@ -5683,7 +6716,7 @@
         <v>10302000</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>9</v>
@@ -5714,7 +6747,7 @@
         <v>10302001</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>9</v>
@@ -5739,7 +6772,7 @@
         <v>10302002</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -5770,7 +6803,7 @@
         <v>10302003</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -5801,7 +6834,7 @@
         <v>10302004</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
@@ -5826,7 +6859,7 @@
         <v>10302005</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -5851,7 +6884,7 @@
         <v>10302006</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
@@ -5882,7 +6915,7 @@
         <v>10302006</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>9</v>
@@ -5907,7 +6940,7 @@
         <v>10303000</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>9</v>
@@ -5944,7 +6977,7 @@
         <v>10304000</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>9</v>
@@ -5975,7 +7008,7 @@
         <v>10305000</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>9</v>
@@ -6010,7 +7043,7 @@
         <v>10401000</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>30</v>
@@ -6043,7 +7076,7 @@
         <v>10401001</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>30</v>
@@ -6070,7 +7103,7 @@
         <v>10401002</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>30</v>
@@ -6103,7 +7136,7 @@
         <v>10402000</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>30</v>
@@ -6138,7 +7171,7 @@
         <v>10402001</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>30</v>
@@ -6173,7 +7206,7 @@
         <v>10402002</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>30</v>
@@ -6208,7 +7241,7 @@
         <v>10402003</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>30</v>
@@ -6237,7 +7270,7 @@
         <v>10402004</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>30</v>
@@ -6272,7 +7305,7 @@
         <v>10402005</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>30</v>
@@ -6301,7 +7334,7 @@
         <v>10402006</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>30</v>
@@ -6336,7 +7369,7 @@
         <v>10402007</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>30</v>
@@ -6365,7 +7398,7 @@
         <v>10402008</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>30</v>
@@ -6400,7 +7433,7 @@
         <v>10402009</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>30</v>
@@ -6435,7 +7468,7 @@
         <v>10402010</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>30</v>
@@ -6470,7 +7503,7 @@
         <v>10402011</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>30</v>
@@ -6505,7 +7538,7 @@
         <v>10402012</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>30</v>
@@ -6534,7 +7567,7 @@
         <v>10402013</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>30</v>
@@ -6569,7 +7602,7 @@
         <v>10402014</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>30</v>
@@ -6598,7 +7631,7 @@
         <v>10403000</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>30</v>
@@ -6637,7 +7670,7 @@
         <v>10501000</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>31</v>
@@ -6672,7 +7705,7 @@
         <v>10502000</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>31</v>
@@ -6701,7 +7734,7 @@
         <v>10503000</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>31</v>
@@ -6738,7 +7771,7 @@
         <v>10504000</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>31</v>
@@ -6769,7 +7802,7 @@
         <v>10505000</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>31</v>
@@ -6804,7 +7837,7 @@
         <v>20101000</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>178</v>
@@ -6826,7 +7859,7 @@
         <v>20102000</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>178</v>
@@ -6849,7 +7882,7 @@
         <v>20201000</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>187</v>
@@ -6882,7 +7915,7 @@
         <v>20202000</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>187</v>
@@ -6915,7 +7948,7 @@
         <v>20203000</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>187</v>
@@ -6954,7 +7987,7 @@
         <v>20204000</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>187</v>
@@ -6993,7 +8026,7 @@
         <v>20205000</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>187</v>
@@ -7028,7 +8061,7 @@
         <v>20301000</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>45</v>
@@ -7061,7 +8094,7 @@
         <v>20302000</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>45</v>
@@ -7096,7 +8129,7 @@
         <v>20302001</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>45</v>
@@ -7131,7 +8164,7 @@
         <v>20302002</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>45</v>
@@ -7166,7 +8199,7 @@
         <v>20303000</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>45</v>
@@ -7201,7 +8234,7 @@
         <v>20304000</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>45</v>
@@ -7228,7 +8261,7 @@
         <v>20305000</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>45</v>
@@ -7261,7 +8294,7 @@
         <v>20305001</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>45</v>
@@ -7292,7 +8325,7 @@
         <v>20305002</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>45</v>
@@ -7323,7 +8356,7 @@
         <v>20306000</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>45</v>
@@ -7360,7 +8393,7 @@
         <v>20307000</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>45</v>
@@ -7397,7 +8430,7 @@
         <v>20401000</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>60</v>
@@ -7424,7 +8457,7 @@
         <v>20401001</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>60</v>
@@ -7457,7 +8490,7 @@
         <v>20402000</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>60</v>
@@ -7486,7 +8519,7 @@
         <v>20403000</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>60</v>
@@ -7515,7 +8548,7 @@
         <v>20404000</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>60</v>
@@ -7544,7 +8577,7 @@
         <v>20501000</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>65</v>
@@ -7577,7 +8610,7 @@
         <v>20501001</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>65</v>
@@ -7610,7 +8643,7 @@
         <v>20501002</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>65</v>
@@ -7643,7 +8676,7 @@
         <v>20502000</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>65</v>
@@ -7670,7 +8703,7 @@
         <v>20502001</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>65</v>
@@ -7697,7 +8730,7 @@
         <v>20502002</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>65</v>
@@ -7724,7 +8757,7 @@
         <v>20503000</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>65</v>
@@ -7757,7 +8790,7 @@
         <v>20503001</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>65</v>
@@ -7790,7 +8823,7 @@
         <v>20503001</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>65</v>
@@ -7823,7 +8856,7 @@
         <v>20601000</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>68</v>
@@ -7856,7 +8889,7 @@
         <v>20602000</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>68</v>
@@ -7889,7 +8922,7 @@
         <v>20603000</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>68</v>
@@ -7922,7 +8955,7 @@
         <v>30101000</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>178</v>
@@ -7945,7 +8978,7 @@
         <v>30102000</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>178</v>
@@ -7968,7 +9001,7 @@
         <v>30201000</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>185</v>
@@ -8001,7 +9034,7 @@
         <v>30202000</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>185</v>
@@ -8034,7 +9067,7 @@
         <v>30203000</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>185</v>
@@ -8067,7 +9100,7 @@
         <v>30204000</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>185</v>
@@ -8102,7 +9135,7 @@
         <v>30205000</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>185</v>
@@ -8133,7 +9166,7 @@
         <v>30206000</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>185</v>
@@ -8170,7 +9203,7 @@
         <v>30207000</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>185</v>
@@ -8207,7 +9240,7 @@
         <v>30208000</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>185</v>
@@ -8240,7 +9273,7 @@
         <v>30209000</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>185</v>
@@ -8265,7 +9298,7 @@
         <v>30301000</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>196</v>
@@ -8294,7 +9327,7 @@
         <v>30401000</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>79</v>
@@ -8327,7 +9360,7 @@
         <v>30401001</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>79</v>
@@ -8360,7 +9393,7 @@
         <v>30401002</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>79</v>
@@ -8387,7 +9420,7 @@
         <v>30401003</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>79</v>
@@ -8414,7 +9447,7 @@
         <v>30401004</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>79</v>
@@ -8447,7 +9480,7 @@
         <v>30401005</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>79</v>
@@ -8474,7 +9507,7 @@
         <v>30401006</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>79</v>
@@ -8507,7 +9540,7 @@
         <v>30401007</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>79</v>
@@ -8540,7 +9573,7 @@
         <v>30401008</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>79</v>
@@ -8573,7 +9606,7 @@
         <v>30401009</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>79</v>
@@ -8600,7 +9633,7 @@
         <v>30402000</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>79</v>
@@ -8633,7 +9666,7 @@
         <v>30403000</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>79</v>
@@ -8666,7 +9699,7 @@
         <v>40101000</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>178</v>
@@ -8689,7 +9722,7 @@
         <v>40102000</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C104" s="14" t="s">
         <v>178</v>
@@ -8712,7 +9745,7 @@
         <v>40201000</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>83</v>
@@ -8747,7 +9780,7 @@
         <v>40301000</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>84</v>
@@ -8782,7 +9815,7 @@
         <v>40302000</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>84</v>
@@ -8819,7 +9852,7 @@
         <v>40303000</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>84</v>
@@ -8854,7 +9887,7 @@
         <v>40401000</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>188</v>
@@ -8883,7 +9916,7 @@
         <v>40402000</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>188</v>
@@ -8918,7 +9951,7 @@
         <v>40403000</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>188</v>
@@ -8951,7 +9984,7 @@
         <v>40403001</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>188</v>
@@ -8978,7 +10011,7 @@
         <v>40404000</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>188</v>
@@ -15894,4 +16927,543 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D947DD-FF6F-4E33-A6C4-4B5832D4473D}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>612</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>607</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D3" t="s">
+        <v>606</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" t="s">
+        <v>600</v>
+      </c>
+      <c r="D4" t="s">
+        <v>605</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D5" t="s">
+        <v>604</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B6" t="s">
+        <v>600</v>
+      </c>
+      <c r="D6" t="s">
+        <v>603</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B7" t="s">
+        <v>600</v>
+      </c>
+      <c r="D7" t="s">
+        <v>602</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>534</v>
+      </c>
+      <c r="B8" t="s">
+        <v>600</v>
+      </c>
+      <c r="D8" t="s">
+        <v>601</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>534</v>
+      </c>
+      <c r="B9" t="s">
+        <v>600</v>
+      </c>
+      <c r="D9" t="s">
+        <v>599</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE884964-8119-4941-9B3D-08527436E9E6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5454A669-0873-45B1-9C27-E6488BB4A9EF}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>612</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>623</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>622</v>
+      </c>
+      <c r="G2" t="s">
+        <v>621</v>
+      </c>
+      <c r="H2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D3" t="s">
+        <v>617</v>
+      </c>
+      <c r="E3">
+        <v>500</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5862DCB-0CAE-485C-9089-B235E3EB4080}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" t="s">
+        <v>627</v>
+      </c>
+      <c r="C3" t="s">
+        <v>601</v>
+      </c>
+      <c r="D3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C4" t="s">
+        <v>601</v>
+      </c>
+      <c r="D4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A51C51E-5097-4C0E-B80A-C20CCA75CC02}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>641</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>600</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>640</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C3" t="s">
+        <v>599</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" t="s">
+        <v>636</v>
+      </c>
+      <c r="C4" t="s">
+        <v>599</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" t="s">
+        <v>635</v>
+      </c>
+      <c r="C5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B6" t="s">
+        <v>634</v>
+      </c>
+      <c r="C6" t="s">
+        <v>599</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B7" t="s">
+        <v>633</v>
+      </c>
+      <c r="C7" t="s">
+        <v>599</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>534</v>
+      </c>
+      <c r="B8" t="s">
+        <v>632</v>
+      </c>
+      <c r="C8" t="s">
+        <v>599</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>